<commit_message>
inicio con las indicaciones del proyecto en cada archivo
</commit_message>
<xml_diff>
--- a/Proyecto 2/Estudio de factibilida POLO360.xlsx
+++ b/Proyecto 2/Estudio de factibilida POLO360.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\PROGRAMADOR WEB INA 2017\PLANIFICACION WEB\1-Planificacion de desarrollo Web\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yoel B\Desktop\Proyecto-2\Proyecto 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="65">
   <si>
     <t>Descripción</t>
   </si>
@@ -205,6 +205,21 @@
   </si>
   <si>
     <t>Alojamiento y dominio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SANDRA </t>
+  </si>
+  <si>
+    <t>ANGELICA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">YOEL </t>
+  </si>
+  <si>
+    <t>POR FAVOR A CRETIVIDAD DE CADA UNA. PUEDEN AGREGAR MAS OPCIONES QUE USTEDES VEAN PERTINENTES A LA HORA DE HACER LOS CAMBIOS.  RECORDANDO QUE TIENE QUE HABER CONCORDANCIA CON LO QUE  EL O LA COMPAÑERA ESCRIBE. EN LA FICHA TECNICA DE LA SIGUIENTE HOJA VA CONFORME AL CRITERIO QUE SE LE ASIGNO .</t>
+  </si>
+  <si>
+    <t>ANADELIS por favor agregar una columna donde aparezcan nuestros nombres usted decide la profesion de cada uno de los integrantes para realizar la hoja de trabajo</t>
   </si>
 </sst>
 </file>
@@ -347,7 +362,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -393,8 +408,32 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="23">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -662,6 +701,15 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF7295D2"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -670,7 +718,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -687,6 +735,82 @@
     <xf numFmtId="0" fontId="6" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="7" fillId="6" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="7" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="2" borderId="6" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="10" fillId="4" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="11" fillId="4" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="18" fillId="3" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="7" fillId="6" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="7" fillId="6" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -705,87 +829,51 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="2" borderId="3" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="2" borderId="4" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="7" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="7" fillId="6" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="7" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="7" fillId="6" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="7" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="7" fillId="6" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="9" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="7" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="7" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="2" fillId="2" borderId="3" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="2" fillId="2" borderId="4" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="2" fillId="2" borderId="6" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="10" fillId="4" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="44" fontId="10" fillId="4" borderId="8" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -798,87 +886,68 @@
     <xf numFmtId="44" fontId="11" fillId="4" borderId="7" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="11" fillId="4" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="18" fillId="3" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1164,10 +1233,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G36"/>
+  <dimension ref="A1:M36"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1178,511 +1247,629 @@
     <col min="7" max="7" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="6" t="s">
+    <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="8"/>
-    </row>
-    <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="33"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="34"/>
+    </row>
+    <row r="3" spans="1:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9" t="s">
+      <c r="C3" s="35"/>
+      <c r="D3" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9" t="s">
+      <c r="E3" s="35"/>
+      <c r="F3" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="10"/>
-    </row>
-    <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G3" s="36"/>
+      <c r="H3" s="76" t="s">
+        <v>64</v>
+      </c>
+      <c r="I3" s="77"/>
+      <c r="J3" s="77"/>
+      <c r="K3" s="77"/>
+    </row>
+    <row r="4" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>1</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="11"/>
-      <c r="D4" s="23">
+      <c r="C4" s="37"/>
+      <c r="D4" s="38">
         <f>(3*5*12)*4000</f>
         <v>720000</v>
       </c>
-      <c r="E4" s="23"/>
-      <c r="F4" s="23">
+      <c r="E4" s="38"/>
+      <c r="F4" s="38">
         <f>D4</f>
         <v>720000</v>
       </c>
-      <c r="G4" s="25"/>
-    </row>
-    <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G4" s="39"/>
+      <c r="H4" s="76"/>
+      <c r="I4" s="77"/>
+      <c r="J4" s="77"/>
+      <c r="K4" s="77"/>
+    </row>
+    <row r="5" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>2</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="13"/>
-      <c r="D5" s="24">
+      <c r="C5" s="29"/>
+      <c r="D5" s="30">
         <f>(3*5*12)*3000</f>
         <v>540000</v>
       </c>
-      <c r="E5" s="24"/>
-      <c r="F5" s="24">
+      <c r="E5" s="30"/>
+      <c r="F5" s="30">
         <f>D5*2</f>
         <v>1080000</v>
       </c>
-      <c r="G5" s="26"/>
-    </row>
-    <row r="6" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G5" s="31"/>
+      <c r="H5" s="76"/>
+      <c r="I5" s="77"/>
+      <c r="J5" s="77"/>
+      <c r="K5" s="77"/>
+    </row>
+    <row r="6" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>1</v>
       </c>
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="13"/>
-      <c r="D6" s="24">
+      <c r="C6" s="29"/>
+      <c r="D6" s="30">
         <f>D4</f>
         <v>720000</v>
       </c>
-      <c r="E6" s="24"/>
-      <c r="F6" s="24">
+      <c r="E6" s="30"/>
+      <c r="F6" s="30">
         <f>D6</f>
         <v>720000</v>
       </c>
-      <c r="G6" s="26"/>
-    </row>
-    <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="15"/>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="27" t="s">
+      <c r="G6" s="31"/>
+      <c r="H6" s="76"/>
+      <c r="I6" s="77"/>
+      <c r="J6" s="77"/>
+      <c r="K6" s="77"/>
+    </row>
+    <row r="7" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="42"/>
+      <c r="B7" s="37"/>
+      <c r="C7" s="37"/>
+      <c r="D7" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="27"/>
-      <c r="F7" s="33">
+      <c r="E7" s="43"/>
+      <c r="F7" s="44">
         <f>SUM(F4:G6)</f>
         <v>2520000</v>
       </c>
-      <c r="G7" s="34"/>
-    </row>
-    <row r="8" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="6" t="s">
+      <c r="G7" s="45"/>
+      <c r="H7" s="76"/>
+      <c r="I7" s="77"/>
+      <c r="J7" s="77"/>
+      <c r="K7" s="77"/>
+    </row>
+    <row r="8" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="8"/>
-    </row>
-    <row r="9" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="17" t="s">
+      <c r="B8" s="33"/>
+      <c r="C8" s="33"/>
+      <c r="D8" s="33"/>
+      <c r="E8" s="33"/>
+      <c r="F8" s="33"/>
+      <c r="G8" s="34"/>
+    </row>
+    <row r="9" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="18"/>
-      <c r="C9" s="18"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="19"/>
-    </row>
-    <row r="10" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="20" t="s">
+      <c r="B9" s="47"/>
+      <c r="C9" s="47"/>
+      <c r="D9" s="47"/>
+      <c r="E9" s="47"/>
+      <c r="F9" s="47"/>
+      <c r="G9" s="48"/>
+    </row>
+    <row r="10" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="49" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="9"/>
-      <c r="C10" s="9" t="s">
+      <c r="B10" s="35"/>
+      <c r="C10" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9" t="s">
+      <c r="D10" s="35"/>
+      <c r="E10" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="F10" s="9"/>
+      <c r="F10" s="35"/>
       <c r="G10" s="5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="21">
+      <c r="H10" s="25" t="s">
+        <v>60</v>
+      </c>
+      <c r="I10" s="26"/>
+    </row>
+    <row r="11" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="40">
         <v>2</v>
       </c>
-      <c r="B11" s="12"/>
-      <c r="C11" s="11" t="s">
+      <c r="B11" s="41"/>
+      <c r="C11" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="11"/>
-      <c r="E11" s="23">
+      <c r="D11" s="37"/>
+      <c r="E11" s="38">
         <v>300</v>
       </c>
-      <c r="F11" s="23"/>
-      <c r="G11" s="28">
+      <c r="F11" s="38"/>
+      <c r="G11" s="6">
         <f>E11*140</f>
         <v>42000</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="22">
+      <c r="H11" s="25"/>
+      <c r="I11" s="26"/>
+      <c r="K11" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="L11" s="24"/>
+      <c r="M11" s="24"/>
+    </row>
+    <row r="12" spans="1:13" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="50">
         <v>1</v>
       </c>
-      <c r="B12" s="14"/>
-      <c r="C12" s="13" t="s">
+      <c r="B12" s="51"/>
+      <c r="C12" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="13"/>
-      <c r="E12" s="24"/>
-      <c r="F12" s="24"/>
-      <c r="G12" s="29">
+      <c r="D12" s="29"/>
+      <c r="E12" s="30"/>
+      <c r="F12" s="30"/>
+      <c r="G12" s="7">
         <f>15*600</f>
         <v>9000</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="17" t="s">
+      <c r="H12" s="25"/>
+      <c r="I12" s="26"/>
+      <c r="K12" s="24"/>
+      <c r="L12" s="24"/>
+      <c r="M12" s="24"/>
+    </row>
+    <row r="13" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="46" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="18"/>
-      <c r="C13" s="18"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="18"/>
-      <c r="G13" s="19"/>
-    </row>
-    <row r="14" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="20" t="s">
+      <c r="B13" s="47"/>
+      <c r="C13" s="47"/>
+      <c r="D13" s="47"/>
+      <c r="E13" s="47"/>
+      <c r="F13" s="47"/>
+      <c r="G13" s="48"/>
+      <c r="H13" s="25"/>
+      <c r="I13" s="26"/>
+      <c r="K13" s="24"/>
+      <c r="L13" s="24"/>
+      <c r="M13" s="24"/>
+    </row>
+    <row r="14" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="49" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="9"/>
-      <c r="C14" s="9" t="s">
+      <c r="B14" s="35"/>
+      <c r="C14" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9" t="s">
+      <c r="D14" s="35"/>
+      <c r="E14" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="F14" s="9"/>
+      <c r="F14" s="35"/>
       <c r="G14" s="5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="21">
+      <c r="H14" s="25"/>
+      <c r="I14" s="26"/>
+      <c r="K14" s="24"/>
+      <c r="L14" s="24"/>
+      <c r="M14" s="24"/>
+    </row>
+    <row r="15" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="40">
         <v>1</v>
       </c>
-      <c r="B15" s="12"/>
-      <c r="C15" s="11" t="s">
+      <c r="B15" s="41"/>
+      <c r="C15" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="D15" s="11"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="16"/>
-      <c r="G15" s="30">
+      <c r="D15" s="37"/>
+      <c r="E15" s="52"/>
+      <c r="F15" s="52"/>
+      <c r="G15" s="8">
         <f>200*600</f>
         <v>120000</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="22"/>
-      <c r="B16" s="14"/>
-      <c r="C16" s="14"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="9" t="s">
+      <c r="H15" s="25"/>
+      <c r="I15" s="26"/>
+      <c r="K15" s="24"/>
+      <c r="L15" s="24"/>
+      <c r="M15" s="24"/>
+    </row>
+    <row r="16" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="50"/>
+      <c r="B16" s="51"/>
+      <c r="C16" s="51"/>
+      <c r="D16" s="51"/>
+      <c r="E16" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="F16" s="9"/>
-      <c r="G16" s="35">
+      <c r="F16" s="35"/>
+      <c r="G16" s="11">
         <f>G11+G12+G15</f>
         <v>171000</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="6" t="s">
+      <c r="H16" s="25"/>
+      <c r="I16" s="26"/>
+      <c r="K16" s="24"/>
+      <c r="L16" s="24"/>
+      <c r="M16" s="24"/>
+    </row>
+    <row r="17" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="8"/>
-    </row>
-    <row r="18" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="20" t="s">
+      <c r="B17" s="33"/>
+      <c r="C17" s="33"/>
+      <c r="D17" s="33"/>
+      <c r="E17" s="33"/>
+      <c r="F17" s="33"/>
+      <c r="G17" s="34"/>
+      <c r="K17" s="24"/>
+      <c r="L17" s="24"/>
+      <c r="M17" s="24"/>
+    </row>
+    <row r="18" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="49" t="s">
         <v>12</v>
       </c>
-      <c r="B18" s="9"/>
-      <c r="C18" s="9" t="s">
+      <c r="B18" s="35"/>
+      <c r="C18" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="D18" s="9"/>
-      <c r="E18" s="9" t="s">
+      <c r="D18" s="35"/>
+      <c r="E18" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="F18" s="9"/>
+      <c r="F18" s="35"/>
       <c r="G18" s="5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="21">
+      <c r="H18" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="I18" s="27"/>
+      <c r="K18" s="24"/>
+      <c r="L18" s="24"/>
+      <c r="M18" s="24"/>
+    </row>
+    <row r="19" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="40">
         <v>1</v>
       </c>
-      <c r="B19" s="12"/>
-      <c r="C19" s="11" t="s">
+      <c r="B19" s="41"/>
+      <c r="C19" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="D19" s="11"/>
-      <c r="E19" s="23">
+      <c r="D19" s="37"/>
+      <c r="E19" s="38">
         <v>1500</v>
       </c>
-      <c r="F19" s="23"/>
-      <c r="G19" s="28">
+      <c r="F19" s="38"/>
+      <c r="G19" s="6">
         <f>E19</f>
         <v>1500</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="22">
+      <c r="H19" s="27"/>
+      <c r="I19" s="27"/>
+      <c r="K19" s="24"/>
+      <c r="L19" s="24"/>
+      <c r="M19" s="24"/>
+    </row>
+    <row r="20" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="50">
         <v>2</v>
       </c>
-      <c r="B20" s="14"/>
-      <c r="C20" s="13" t="s">
+      <c r="B20" s="51"/>
+      <c r="C20" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="D20" s="13"/>
-      <c r="E20" s="24">
+      <c r="D20" s="29"/>
+      <c r="E20" s="30">
         <v>10000</v>
       </c>
-      <c r="F20" s="24"/>
-      <c r="G20" s="31">
+      <c r="F20" s="30"/>
+      <c r="G20" s="9">
         <f>E20*A20</f>
         <v>20000</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="21">
+      <c r="H20" s="27"/>
+      <c r="I20" s="27"/>
+      <c r="K20" s="24"/>
+      <c r="L20" s="24"/>
+      <c r="M20" s="24"/>
+    </row>
+    <row r="21" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="40">
         <f>10*12</f>
         <v>120</v>
       </c>
-      <c r="B21" s="12"/>
-      <c r="C21" s="11" t="s">
+      <c r="B21" s="41"/>
+      <c r="C21" s="37" t="s">
         <v>22</v>
       </c>
-      <c r="D21" s="11"/>
-      <c r="E21" s="23">
+      <c r="D21" s="37"/>
+      <c r="E21" s="38">
         <v>300</v>
       </c>
-      <c r="F21" s="23"/>
-      <c r="G21" s="32">
+      <c r="F21" s="38"/>
+      <c r="G21" s="10">
         <f>E21*A21</f>
         <v>36000</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="22">
+      <c r="H21" s="27"/>
+      <c r="I21" s="27"/>
+      <c r="K21" s="24"/>
+      <c r="L21" s="24"/>
+      <c r="M21" s="24"/>
+    </row>
+    <row r="22" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="50">
         <f>60*4</f>
         <v>240</v>
       </c>
-      <c r="B22" s="14"/>
-      <c r="C22" s="13" t="s">
+      <c r="B22" s="51"/>
+      <c r="C22" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="D22" s="13"/>
-      <c r="E22" s="24">
+      <c r="D22" s="29"/>
+      <c r="E22" s="30">
         <v>5000</v>
       </c>
-      <c r="F22" s="24"/>
-      <c r="G22" s="31">
+      <c r="F22" s="30"/>
+      <c r="G22" s="9">
         <f>E22*A22</f>
         <v>1200000</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="21"/>
-      <c r="B23" s="12"/>
-      <c r="C23" s="12"/>
-      <c r="D23" s="12"/>
-      <c r="E23" s="16" t="s">
+      <c r="H22" s="27"/>
+      <c r="I22" s="27"/>
+      <c r="K22" s="24"/>
+      <c r="L22" s="24"/>
+      <c r="M22" s="24"/>
+    </row>
+    <row r="23" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="40"/>
+      <c r="B23" s="41"/>
+      <c r="C23" s="41"/>
+      <c r="D23" s="41"/>
+      <c r="E23" s="52" t="s">
         <v>9</v>
       </c>
-      <c r="F23" s="16"/>
-      <c r="G23" s="35">
+      <c r="F23" s="52"/>
+      <c r="G23" s="11">
         <f>SUM(G19:G22)</f>
         <v>1257500</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="36"/>
-      <c r="B24" s="37"/>
-      <c r="C24" s="37"/>
-      <c r="D24" s="37"/>
-      <c r="E24" s="39" t="s">
+      <c r="H23" s="27"/>
+      <c r="I23" s="27"/>
+    </row>
+    <row r="24" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="12"/>
+      <c r="B24" s="13"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="53" t="s">
         <v>26</v>
       </c>
-      <c r="F24" s="40"/>
-      <c r="G24" s="38">
+      <c r="F24" s="54"/>
+      <c r="G24" s="14">
         <f>SUM(G23,G16,F7)</f>
         <v>3948500</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="6" t="s">
+      <c r="H24" s="27"/>
+      <c r="I24" s="27"/>
+    </row>
+    <row r="25" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="B25" s="7"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="7"/>
-      <c r="E25" s="7"/>
-      <c r="F25" s="7"/>
-      <c r="G25" s="8"/>
-    </row>
-    <row r="26" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="20" t="s">
+      <c r="B25" s="33"/>
+      <c r="C25" s="33"/>
+      <c r="D25" s="33"/>
+      <c r="E25" s="33"/>
+      <c r="F25" s="33"/>
+      <c r="G25" s="34"/>
+    </row>
+    <row r="26" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="49" t="s">
         <v>12</v>
       </c>
-      <c r="B26" s="9"/>
-      <c r="C26" s="9" t="s">
+      <c r="B26" s="35"/>
+      <c r="C26" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="D26" s="9"/>
-      <c r="E26" s="9" t="s">
+      <c r="D26" s="35"/>
+      <c r="E26" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="F26" s="9"/>
+      <c r="F26" s="35"/>
       <c r="G26" s="5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="21">
+      <c r="H26" s="28" t="s">
+        <v>62</v>
+      </c>
+      <c r="I26" s="28"/>
+    </row>
+    <row r="27" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="40">
         <v>1</v>
       </c>
-      <c r="B27" s="12"/>
-      <c r="C27" s="11" t="s">
+      <c r="B27" s="41"/>
+      <c r="C27" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="D27" s="11"/>
-      <c r="E27" s="23"/>
-      <c r="F27" s="23"/>
-      <c r="G27" s="28">
+      <c r="D27" s="37"/>
+      <c r="E27" s="38"/>
+      <c r="F27" s="38"/>
+      <c r="G27" s="6">
         <f>G24*0.1</f>
         <v>394850</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="29" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="6" t="s">
+      <c r="H27" s="28"/>
+      <c r="I27" s="28"/>
+    </row>
+    <row r="28" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H28" s="28"/>
+      <c r="I28" s="28"/>
+    </row>
+    <row r="29" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="B29" s="7"/>
-      <c r="C29" s="7"/>
-      <c r="D29" s="7"/>
-      <c r="E29" s="7"/>
-      <c r="F29" s="7"/>
-      <c r="G29" s="8"/>
-    </row>
-    <row r="30" spans="1:7" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="36"/>
-      <c r="B30" s="37"/>
-      <c r="C30" s="37"/>
-      <c r="D30" s="37"/>
-      <c r="E30" s="41" t="s">
+      <c r="B29" s="33"/>
+      <c r="C29" s="33"/>
+      <c r="D29" s="33"/>
+      <c r="E29" s="33"/>
+      <c r="F29" s="33"/>
+      <c r="G29" s="34"/>
+      <c r="H29" s="28"/>
+      <c r="I29" s="28"/>
+    </row>
+    <row r="30" spans="1:13" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="12"/>
+      <c r="B30" s="13"/>
+      <c r="C30" s="13"/>
+      <c r="D30" s="13"/>
+      <c r="E30" s="55" t="s">
         <v>28</v>
       </c>
-      <c r="F30" s="42"/>
-      <c r="G30" s="43">
+      <c r="F30" s="56"/>
+      <c r="G30" s="15">
         <f>G24+G27</f>
         <v>4343350</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="32" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="68" t="s">
+      <c r="H30" s="28"/>
+      <c r="I30" s="28"/>
+    </row>
+    <row r="31" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H31" s="28"/>
+      <c r="I31" s="28"/>
+    </row>
+    <row r="32" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="57" t="s">
         <v>56</v>
       </c>
-      <c r="B32" s="69"/>
-      <c r="C32" s="69"/>
-      <c r="D32" s="69"/>
-      <c r="E32" s="69"/>
-      <c r="F32" s="69"/>
-      <c r="G32" s="70"/>
-    </row>
-    <row r="33" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="20" t="s">
+      <c r="B32" s="58"/>
+      <c r="C32" s="58"/>
+      <c r="D32" s="58"/>
+      <c r="E32" s="58"/>
+      <c r="F32" s="58"/>
+      <c r="G32" s="59"/>
+      <c r="H32" s="28"/>
+      <c r="I32" s="28"/>
+    </row>
+    <row r="33" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="49" t="s">
         <v>12</v>
       </c>
-      <c r="B33" s="9"/>
-      <c r="C33" s="9" t="s">
+      <c r="B33" s="35"/>
+      <c r="C33" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="D33" s="9"/>
-      <c r="E33" s="9" t="s">
+      <c r="D33" s="35"/>
+      <c r="E33" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="F33" s="9"/>
+      <c r="F33" s="35"/>
       <c r="G33" s="5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="21">
+      <c r="H33" s="28"/>
+      <c r="I33" s="28"/>
+    </row>
+    <row r="34" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="40">
         <v>1</v>
       </c>
-      <c r="B34" s="12"/>
-      <c r="C34" s="11" t="s">
+      <c r="B34" s="41"/>
+      <c r="C34" s="37" t="s">
         <v>57</v>
       </c>
-      <c r="D34" s="11"/>
-      <c r="E34" s="23"/>
-      <c r="F34" s="23"/>
-      <c r="G34" s="28">
+      <c r="D34" s="37"/>
+      <c r="E34" s="38"/>
+      <c r="F34" s="38"/>
+      <c r="G34" s="6">
         <f>100*600</f>
         <v>60000</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="21">
+      <c r="H34" s="28"/>
+      <c r="I34" s="28"/>
+    </row>
+    <row r="35" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="40">
         <v>1</v>
       </c>
-      <c r="B35" s="12"/>
-      <c r="C35" s="11" t="s">
+      <c r="B35" s="41"/>
+      <c r="C35" s="37" t="s">
         <v>58</v>
       </c>
-      <c r="D35" s="11"/>
-      <c r="E35" s="23"/>
-      <c r="F35" s="23"/>
-      <c r="G35" s="28">
+      <c r="D35" s="37"/>
+      <c r="E35" s="38"/>
+      <c r="F35" s="38"/>
+      <c r="G35" s="6">
         <f>120*600</f>
         <v>72000</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D36" s="66" t="s">
+      <c r="H35" s="28"/>
+      <c r="I35" s="28"/>
+    </row>
+    <row r="36" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D36" s="60" t="s">
         <v>59</v>
       </c>
-      <c r="E36" s="66"/>
-      <c r="F36" s="66"/>
-      <c r="G36" s="67">
+      <c r="E36" s="60"/>
+      <c r="F36" s="60"/>
+      <c r="G36" s="23">
         <f>SUM(G34:G35)</f>
         <v>132000</v>
       </c>
+      <c r="H36" s="28"/>
+      <c r="I36" s="28"/>
     </row>
   </sheetData>
-  <mergeCells count="75">
+  <mergeCells count="80">
     <mergeCell ref="D36:F36"/>
     <mergeCell ref="A34:B34"/>
     <mergeCell ref="C34:D34"/>
@@ -1702,11 +1889,6 @@
     <mergeCell ref="A27:B27"/>
     <mergeCell ref="C27:D27"/>
     <mergeCell ref="E27:F27"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="A23:D23"/>
-    <mergeCell ref="E23:F23"/>
     <mergeCell ref="A25:G25"/>
     <mergeCell ref="E24:F24"/>
     <mergeCell ref="A20:B20"/>
@@ -1715,17 +1897,17 @@
     <mergeCell ref="A21:B21"/>
     <mergeCell ref="C21:D21"/>
     <mergeCell ref="E21:F21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="A23:D23"/>
+    <mergeCell ref="E23:F23"/>
     <mergeCell ref="A18:B18"/>
     <mergeCell ref="C18:D18"/>
     <mergeCell ref="E18:F18"/>
     <mergeCell ref="A19:B19"/>
     <mergeCell ref="C19:D19"/>
     <mergeCell ref="E19:F19"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="A16:D16"/>
-    <mergeCell ref="E16:F16"/>
     <mergeCell ref="A17:G17"/>
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="C12:D12"/>
@@ -1734,11 +1916,11 @@
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="C14:D14"/>
     <mergeCell ref="E14:F14"/>
-    <mergeCell ref="A8:G8"/>
-    <mergeCell ref="A9:G9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="A16:D16"/>
+    <mergeCell ref="E16:F16"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="C11:D11"/>
     <mergeCell ref="E11:F11"/>
@@ -1748,6 +1930,11 @@
     <mergeCell ref="A7:C7"/>
     <mergeCell ref="D7:E7"/>
     <mergeCell ref="F7:G7"/>
+    <mergeCell ref="A8:G8"/>
+    <mergeCell ref="A9:G9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="E10:F10"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="D5:E5"/>
     <mergeCell ref="F5:G5"/>
@@ -1758,6 +1945,11 @@
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="D4:E4"/>
     <mergeCell ref="F4:G4"/>
+    <mergeCell ref="K11:M22"/>
+    <mergeCell ref="H10:I16"/>
+    <mergeCell ref="H18:I24"/>
+    <mergeCell ref="H26:I36"/>
+    <mergeCell ref="H3:K7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967294" verticalDpi="4294967294" r:id="rId1"/>
@@ -1768,7 +1960,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A13" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="A18" sqref="A18:D19"/>
     </sheetView>
   </sheetViews>
@@ -1780,218 +1972,218 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="67" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="51"/>
-      <c r="C1" s="51"/>
-      <c r="D1" s="52"/>
+      <c r="B1" s="68"/>
+      <c r="C1" s="68"/>
+      <c r="D1" s="69"/>
       <c r="E1" s="3"/>
     </row>
     <row r="2" spans="1:5" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="65" t="s">
+      <c r="A2" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="65" t="s">
+      <c r="B2" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="65" t="s">
+      <c r="C2" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="65" t="s">
+      <c r="D2" s="22" t="s">
         <v>12</v>
       </c>
       <c r="E2" s="3"/>
     </row>
-    <row r="3" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="44" t="s">
+    <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="53" t="s">
+      <c r="B3" s="70" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="46" t="s">
+      <c r="C3" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="D3" s="47">
+      <c r="D3" s="19">
         <v>2</v>
       </c>
       <c r="E3" s="3"/>
     </row>
-    <row r="4" spans="1:5" ht="86.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="44" t="s">
+    <row r="4" spans="1:5" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="54"/>
-      <c r="C4" s="46" t="s">
+      <c r="B4" s="71"/>
+      <c r="C4" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="D4" s="47">
+      <c r="D4" s="19">
         <v>1</v>
       </c>
       <c r="E4" s="3"/>
     </row>
     <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="45"/>
-      <c r="B5" s="55"/>
-      <c r="C5" s="46" t="s">
+      <c r="A5" s="17"/>
+      <c r="B5" s="72"/>
+      <c r="C5" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="D5" s="47">
+      <c r="D5" s="19">
         <v>1</v>
       </c>
       <c r="E5" s="3"/>
     </row>
-    <row r="6" spans="1:5" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="56" t="s">
+    <row r="6" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="73" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="53" t="s">
+      <c r="B6" s="70" t="s">
         <v>38</v>
       </c>
-      <c r="C6" s="46" t="s">
+      <c r="C6" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="D6" s="47">
+      <c r="D6" s="19">
         <v>1</v>
       </c>
       <c r="E6" s="3"/>
     </row>
-    <row r="7" spans="1:5" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="57"/>
-      <c r="B7" s="54"/>
-      <c r="C7" s="48" t="s">
+    <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="74"/>
+      <c r="B7" s="71"/>
+      <c r="C7" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="D7" s="53"/>
+      <c r="D7" s="70"/>
       <c r="E7" s="3"/>
     </row>
     <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="57"/>
-      <c r="B8" s="54"/>
-      <c r="C8" s="49" t="s">
+      <c r="A8" s="74"/>
+      <c r="B8" s="71"/>
+      <c r="C8" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="D8" s="54"/>
+      <c r="D8" s="71"/>
       <c r="E8" s="3"/>
     </row>
     <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="57"/>
-      <c r="B9" s="55"/>
-      <c r="C9" s="49" t="s">
+      <c r="A9" s="74"/>
+      <c r="B9" s="72"/>
+      <c r="C9" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="D9" s="55"/>
+      <c r="D9" s="72"/>
       <c r="E9" s="3"/>
     </row>
     <row r="10" spans="1:5" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="58"/>
-      <c r="B10" s="47" t="s">
+      <c r="A10" s="75"/>
+      <c r="B10" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="C10" s="46" t="s">
+      <c r="C10" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="D10" s="47">
+      <c r="D10" s="19">
         <v>1</v>
       </c>
       <c r="E10" s="3"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="56" t="s">
+      <c r="A11" s="73" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="53" t="s">
+      <c r="B11" s="70" t="s">
         <v>53</v>
       </c>
-      <c r="C11" s="53" t="s">
+      <c r="C11" s="70" t="s">
         <v>54</v>
       </c>
-      <c r="D11" s="53">
+      <c r="D11" s="70">
         <v>3</v>
       </c>
       <c r="E11" s="3"/>
     </row>
     <row r="12" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="57"/>
-      <c r="B12" s="55"/>
-      <c r="C12" s="55"/>
-      <c r="D12" s="55"/>
+      <c r="A12" s="74"/>
+      <c r="B12" s="72"/>
+      <c r="C12" s="72"/>
+      <c r="D12" s="72"/>
       <c r="E12" s="3"/>
     </row>
     <row r="13" spans="1:5" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="57"/>
-      <c r="B13" s="47" t="s">
+      <c r="A13" s="74"/>
+      <c r="B13" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="C13" s="46" t="s">
+      <c r="C13" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="D13" s="47">
+      <c r="D13" s="19">
         <v>3</v>
       </c>
       <c r="E13" s="3"/>
     </row>
     <row r="14" spans="1:5" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="57"/>
-      <c r="B14" s="47" t="s">
+      <c r="A14" s="74"/>
+      <c r="B14" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="C14" s="46" t="s">
+      <c r="C14" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="D14" s="47">
+      <c r="D14" s="19">
         <v>1</v>
       </c>
       <c r="E14" s="3"/>
     </row>
     <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="57"/>
-      <c r="B15" s="46" t="s">
+      <c r="A15" s="74"/>
+      <c r="B15" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="C15" s="46" t="s">
+      <c r="C15" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="D15" s="47">
+      <c r="D15" s="19">
         <v>1</v>
       </c>
       <c r="E15" s="3"/>
     </row>
     <row r="16" spans="1:5" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="57"/>
-      <c r="B16" s="60" t="s">
+      <c r="A16" s="74"/>
+      <c r="B16" s="61" t="s">
         <v>48</v>
       </c>
       <c r="C16" s="62" t="s">
         <v>49</v>
       </c>
-      <c r="D16" s="64">
+      <c r="D16" s="63">
         <v>1</v>
       </c>
       <c r="E16" s="3"/>
     </row>
     <row r="17" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="58"/>
-      <c r="B17" s="61"/>
-      <c r="C17" s="63"/>
-      <c r="D17" s="59"/>
+      <c r="A17" s="75"/>
+      <c r="B17" s="64"/>
+      <c r="C17" s="65"/>
+      <c r="D17" s="66"/>
       <c r="E17" s="3"/>
     </row>
     <row r="18" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="60" t="s">
+      <c r="A18" s="61" t="s">
         <v>50</v>
       </c>
       <c r="B18" s="62"/>
       <c r="C18" s="62"/>
-      <c r="D18" s="64"/>
+      <c r="D18" s="63"/>
       <c r="E18" s="3"/>
     </row>
     <row r="19" spans="1:5" ht="59.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="61"/>
-      <c r="B19" s="63"/>
-      <c r="C19" s="63"/>
-      <c r="D19" s="59"/>
+      <c r="A19" s="64"/>
+      <c r="B19" s="65"/>
+      <c r="C19" s="65"/>
+      <c r="D19" s="66"/>
       <c r="E19" s="3"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -1999,12 +2191,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="D16:D17"/>
     <mergeCell ref="A18:D19"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="B3:B5"/>
@@ -2012,6 +2198,12 @@
     <mergeCell ref="B6:B9"/>
     <mergeCell ref="D7:D9"/>
     <mergeCell ref="A11:A17"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="D16:D17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967294" verticalDpi="4294967294" r:id="rId1"/>

</xml_diff>